<commit_message>
Started with the uniform. critical-like, symmetric and octave designs
</commit_message>
<xml_diff>
--- a/Report/Tables.xlsx
+++ b/Report/Tables.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Daniel\Varsity\4th Year\Design Project\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Daniel\Varsity\4th Year\Design Project\Adaptive_Hearing_Aid\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA2A978-A221-4F96-BF7F-83D5DE6673B3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A3FBE5-71CD-42AE-91A9-0D2EE8AD63FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{0BB7CC49-5138-4F42-AF03-7B48BFE4C146}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="5" xr2:uid="{0BB7CC49-5138-4F42-AF03-7B48BFE4C146}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Insertion Gain ParametersFre" sheetId="2" r:id="rId2"/>
+    <sheet name="Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Bark Scale" sheetId="4" r:id="rId4"/>
+    <sheet name="Symmetric" sheetId="5" r:id="rId5"/>
+    <sheet name="Octave" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="63">
   <si>
     <t>Filter Specifications</t>
   </si>
@@ -178,6 +182,48 @@
   </si>
   <si>
     <t>ki (dB)</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Filters </t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center Frequency (Hz) </t>
+  </si>
+  <si>
+    <t>Cut-Off Frequency (Hz)</t>
+  </si>
+  <si>
+    <t>Bandwidth (Hz)</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Band Number</t>
+  </si>
+  <si>
+    <t>Lower Passband Frequency</t>
+  </si>
+  <si>
+    <t>Upper Passband Frequency</t>
+  </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>Center Frequency (Hz)</t>
+  </si>
+  <si>
+    <t>Lower Passband Frequency (Hz)</t>
+  </si>
+  <si>
+    <t>Upper Passband Frequency (Hz)</t>
   </si>
 </sst>
 </file>
@@ -209,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -232,18 +278,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA0B17E-73E0-4EF2-943B-8C385AD95F0C}">
   <dimension ref="A1:BH9"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="AX21" sqref="AX21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,140 +679,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BA1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BD1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BE1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BG1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BH1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1592,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DED8EAB-8A02-4BEB-B55A-E8CDAC599B2C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,4 +1728,1139 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8142D730-A3F2-41C7-942E-EFD0188BC00B}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7AB1D2-0A19-4C00-9AAC-39A308A7EAD4}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>80</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>60</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+      <c r="J3" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1">
+        <v>200</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>150</v>
+      </c>
+      <c r="I4" s="1">
+        <v>200</v>
+      </c>
+      <c r="J4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>250</v>
+      </c>
+      <c r="C5" s="1">
+        <v>300</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>250</v>
+      </c>
+      <c r="I5" s="1">
+        <v>300</v>
+      </c>
+      <c r="J5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>350</v>
+      </c>
+      <c r="C6" s="1">
+        <v>400</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>350</v>
+      </c>
+      <c r="I6" s="1">
+        <v>400</v>
+      </c>
+      <c r="J6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>450</v>
+      </c>
+      <c r="C7" s="1">
+        <v>510</v>
+      </c>
+      <c r="D7" s="1">
+        <v>110</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>450</v>
+      </c>
+      <c r="I7" s="1">
+        <v>510</v>
+      </c>
+      <c r="J7" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>570</v>
+      </c>
+      <c r="C8" s="1">
+        <v>630</v>
+      </c>
+      <c r="D8" s="1">
+        <v>120</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>570</v>
+      </c>
+      <c r="I8" s="1">
+        <v>630</v>
+      </c>
+      <c r="J8" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>700</v>
+      </c>
+      <c r="C9" s="1">
+        <v>770</v>
+      </c>
+      <c r="D9" s="1">
+        <v>140</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>700</v>
+      </c>
+      <c r="I9" s="1">
+        <v>770</v>
+      </c>
+      <c r="J9" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>840</v>
+      </c>
+      <c r="C10" s="1">
+        <v>920</v>
+      </c>
+      <c r="D10" s="1">
+        <v>150</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="1">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>840</v>
+      </c>
+      <c r="I10" s="1">
+        <v>920</v>
+      </c>
+      <c r="J10" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1080</v>
+      </c>
+      <c r="D11" s="1">
+        <v>160</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1080</v>
+      </c>
+      <c r="J11" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1170</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1270</v>
+      </c>
+      <c r="D12" s="1">
+        <v>190</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1170</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1270</v>
+      </c>
+      <c r="J12" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1370</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1480</v>
+      </c>
+      <c r="D13" s="1">
+        <v>210</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1370</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1480</v>
+      </c>
+      <c r="J13" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1720</v>
+      </c>
+      <c r="D14" s="1">
+        <v>240</v>
+      </c>
+      <c r="F14" s="5">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1600</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1720</v>
+      </c>
+      <c r="J14" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1850</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D15" s="1">
+        <v>280</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1850</v>
+      </c>
+      <c r="I15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J15" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2320</v>
+      </c>
+      <c r="D16" s="1">
+        <v>320</v>
+      </c>
+      <c r="F16" s="5">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2150</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2320</v>
+      </c>
+      <c r="J16" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D17" s="1">
+        <v>380</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="1">
+        <v>15</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2500</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2700</v>
+      </c>
+      <c r="J17" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2900</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3150</v>
+      </c>
+      <c r="D18" s="1">
+        <v>450</v>
+      </c>
+      <c r="F18" s="5">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2900</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3150</v>
+      </c>
+      <c r="J18" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3400</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3700</v>
+      </c>
+      <c r="D19" s="1">
+        <v>550</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="1">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3400</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3700</v>
+      </c>
+      <c r="J19" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4000</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4400</v>
+      </c>
+      <c r="D20" s="1">
+        <v>700</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1">
+        <v>18</v>
+      </c>
+      <c r="H20" s="1">
+        <v>4000</v>
+      </c>
+      <c r="I20" s="1">
+        <v>4400</v>
+      </c>
+      <c r="J20" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4800</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5300</v>
+      </c>
+      <c r="D21" s="1">
+        <v>900</v>
+      </c>
+      <c r="F21" s="5">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1">
+        <v>19</v>
+      </c>
+      <c r="H21" s="1">
+        <v>4800</v>
+      </c>
+      <c r="I21" s="1">
+        <v>5300</v>
+      </c>
+      <c r="J21" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5800</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6400</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1100</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="1">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1">
+        <v>5800</v>
+      </c>
+      <c r="I22" s="1">
+        <v>6400</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>7000</v>
+      </c>
+      <c r="C23" s="1">
+        <v>7700</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1300</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="1">
+        <v>21</v>
+      </c>
+      <c r="H23" s="1">
+        <v>7000</v>
+      </c>
+      <c r="I23" s="1">
+        <v>7700</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8500</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9500</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10500</v>
+      </c>
+      <c r="C25" s="1">
+        <v>12000</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>13500</v>
+      </c>
+      <c r="C26" s="1">
+        <v>15500</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EFE3E3-C957-471B-AE8B-36918DB0CCF0}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>500</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2-B2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D9" si="0">C3-B3</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7500</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7500</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0711990E-69C1-490E-9831-9A270016A4DF}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <f>(B2)/(2^(0.5))</f>
+        <v>44.547727214752491</v>
+      </c>
+      <c r="D2">
+        <f>(2^(0.5))*(B2)</f>
+        <v>89.095454429504997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C9" si="0">(B3)/(2^(0.5))</f>
+        <v>88.38834764831843</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" si="1">(2^(0.5))*(B3)</f>
+        <v>176.77669529663689</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>176.77669529663686</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>353.55339059327378</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>353.55339059327372</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>707.10678118654755</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>707.10678118654744</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1414.2135623730951</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1414.2135623730949</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2828.4271247461902</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2828.4271247461897</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>5656.8542494923804</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8000</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5656.8542494923795</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>11313.708498984761</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on dynamic compression
</commit_message>
<xml_diff>
--- a/Report/Tables.xlsx
+++ b/Report/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Daniel\Varsity\4th Year\Design Project\Adaptive_Hearing_Aid\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C07E76-515F-449B-97B9-5E371ABC5E57}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F59DFD-168E-4C90-A3E1-CD6A3A79A92F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="3" activeTab="10" xr2:uid="{0BB7CC49-5138-4F42-AF03-7B48BFE4C146}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="10" xr2:uid="{0BB7CC49-5138-4F42-AF03-7B48BFE4C146}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter Parameters" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="ANSI" sheetId="9" r:id="rId9"/>
     <sheet name="ANSI new" sheetId="11" r:id="rId10"/>
     <sheet name="ANSI Oct" sheetId="10" r:id="rId11"/>
+    <sheet name="Compression" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="95">
   <si>
     <t>Filter Specifications</t>
   </si>
@@ -295,6 +296,36 @@
   </si>
   <si>
     <t>Upper Stopband Frequency</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Control (Input or Output)</t>
+  </si>
+  <si>
+    <t>Compression Threshold</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Compression Ratio</t>
+  </si>
+  <si>
+    <t>Attack/Release Time</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Number of Channels</t>
+  </si>
+  <si>
+    <t>Multiple</t>
   </si>
 </sst>
 </file>
@@ -2709,7 +2740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomLeft" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,6 +3775,77 @@
     <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81EF629-05BF-4800-8BE8-A7D2F3A82A32}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>